<commit_message>
fix: name details in brackets
</commit_message>
<xml_diff>
--- a/data/pokemon_dex_hisui_paldea.xlsx
+++ b/data/pokemon_dex_hisui_paldea.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\panpa\Google Drive\Data science\pkmr\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB8AF94-E86D-4141-AABF-45FAC1E32F92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30D6C972-5198-40FD-8FDC-EEF954163001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="825" yWindow="-120" windowWidth="19785" windowHeight="11760" xr2:uid="{B1A15022-E2F9-4772-961C-F274C4B8A95E}"/>
+    <workbookView xWindow="1245" yWindow="30" windowWidth="19245" windowHeight="11490" xr2:uid="{B1A15022-E2F9-4772-961C-F274C4B8A95E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -584,51 +584,6 @@
     <t>Gholdengo</t>
   </si>
   <si>
-    <t>Maushold Additional Form @</t>
-  </si>
-  <si>
-    <t>Palafin Base Form @</t>
-  </si>
-  <si>
-    <t>Oinkologne Male Form @</t>
-  </si>
-  <si>
-    <t>Oinkologne Female Form @</t>
-  </si>
-  <si>
-    <t>Dudunsparce Two-segment @</t>
-  </si>
-  <si>
-    <t>Dudunsparce Three-segment @</t>
-  </si>
-  <si>
-    <t>Palafin Hero Form @</t>
-  </si>
-  <si>
-    <t>Maushold Base Form @</t>
-  </si>
-  <si>
-    <t>Tatsugiri Colour1 @</t>
-  </si>
-  <si>
-    <t>Tatsugiri Colour2 @</t>
-  </si>
-  <si>
-    <t>Tatsugiri Colour3 @</t>
-  </si>
-  <si>
-    <t>Squawkabilly Colour1 @</t>
-  </si>
-  <si>
-    <t>Squawkabilly Colour2 @</t>
-  </si>
-  <si>
-    <t>Squawkabilly Colour3 @</t>
-  </si>
-  <si>
-    <t>Squawkabilly Colour4 @</t>
-  </si>
-  <si>
     <t>Gimmighoul (Chest Form)</t>
   </si>
   <si>
@@ -702,6 +657,51 @@
   </si>
   <si>
     <t>Chi-Yu (Fish)</t>
+  </si>
+  <si>
+    <t>Oinkologne (Male Form @)</t>
+  </si>
+  <si>
+    <t>Oinkologne (Female Form @)</t>
+  </si>
+  <si>
+    <t>Dudunsparce (Two-segment @)</t>
+  </si>
+  <si>
+    <t>Dudunsparce (Three-segment @)</t>
+  </si>
+  <si>
+    <t>Palafin (Base Form @)</t>
+  </si>
+  <si>
+    <t>Palafin (Hero Form @)</t>
+  </si>
+  <si>
+    <t>Maushold (Base Form @)</t>
+  </si>
+  <si>
+    <t>Maushold (Additional Form @)</t>
+  </si>
+  <si>
+    <t>Tatsugiri (Colour1 @)</t>
+  </si>
+  <si>
+    <t>Tatsugiri (Colour2 @)</t>
+  </si>
+  <si>
+    <t>Tatsugiri (Colour3 @)</t>
+  </si>
+  <si>
+    <t>Squawkabilly (Colour1 @)</t>
+  </si>
+  <si>
+    <t>Squawkabilly (Colour2 @)</t>
+  </si>
+  <si>
+    <t>Squawkabilly (Colour3 @)</t>
+  </si>
+  <si>
+    <t>Squawkabilly (Colour4 @)</t>
   </si>
 </sst>
 </file>
@@ -1054,8 +1054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5180E553-97C3-4D11-A13B-DD8E8ABEE531}">
   <dimension ref="A1:Q148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="G112" sqref="G112"/>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="C93" sqref="C93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1114,10 +1114,10 @@
         <v>10</v>
       </c>
       <c r="P1" t="s">
-        <v>216</v>
+        <v>201</v>
       </c>
       <c r="Q1" t="s">
-        <v>217</v>
+        <v>202</v>
       </c>
     </row>
     <row r="2" spans="1:17">
@@ -1164,7 +1164,7 @@
         <v>90</v>
       </c>
       <c r="P2" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -1211,7 +1211,7 @@
         <v>120</v>
       </c>
       <c r="P3" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -1261,7 +1261,7 @@
         <v>50</v>
       </c>
       <c r="P4" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -1361,7 +1361,7 @@
         <v>50</v>
       </c>
       <c r="P6" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -1411,7 +1411,7 @@
         <v>50</v>
       </c>
       <c r="P7" t="s">
-        <v>211</v>
+        <v>196</v>
       </c>
     </row>
     <row r="8" spans="1:17">
@@ -1461,7 +1461,7 @@
         <v>50</v>
       </c>
       <c r="P8" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -1511,7 +1511,7 @@
         <v>50</v>
       </c>
       <c r="P9" t="s">
-        <v>211</v>
+        <v>196</v>
       </c>
     </row>
     <row r="10" spans="1:17">
@@ -1561,7 +1561,7 @@
         <v>0</v>
       </c>
       <c r="P10" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
     </row>
     <row r="11" spans="1:17">
@@ -1611,7 +1611,7 @@
         <v>0</v>
       </c>
       <c r="P11" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
     </row>
     <row r="12" spans="1:17">
@@ -1661,7 +1661,7 @@
         <v>75</v>
       </c>
       <c r="P12" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
     </row>
     <row r="13" spans="1:17">
@@ -1711,7 +1711,7 @@
         <v>75</v>
       </c>
       <c r="P13" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
     </row>
     <row r="14" spans="1:17">
@@ -1758,7 +1758,7 @@
         <v>100</v>
       </c>
       <c r="P14" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
     </row>
     <row r="15" spans="1:17">
@@ -1805,7 +1805,7 @@
         <v>150</v>
       </c>
       <c r="P15" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
     </row>
     <row r="16" spans="1:17">
@@ -1855,7 +1855,7 @@
         <v>87.5</v>
       </c>
       <c r="P16" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
     </row>
     <row r="17" spans="1:17">
@@ -1905,7 +1905,7 @@
         <v>50</v>
       </c>
       <c r="P17" t="s">
-        <v>211</v>
+        <v>196</v>
       </c>
     </row>
     <row r="18" spans="1:17">
@@ -1955,7 +1955,7 @@
         <v>50</v>
       </c>
       <c r="P18" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
     </row>
     <row r="19" spans="1:17">
@@ -2005,7 +2005,7 @@
         <v>87.5</v>
       </c>
       <c r="P19" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
     </row>
     <row r="20" spans="1:17">
@@ -2102,7 +2102,7 @@
         <v>50</v>
       </c>
       <c r="P21" t="s">
-        <v>211</v>
+        <v>196</v>
       </c>
     </row>
     <row r="22" spans="1:17">
@@ -2152,7 +2152,7 @@
         <v>87.5</v>
       </c>
       <c r="P22" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
     </row>
     <row r="23" spans="1:17">
@@ -2202,7 +2202,7 @@
         <v>87.5</v>
       </c>
       <c r="P23" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
     </row>
     <row r="24" spans="1:17">
@@ -2402,10 +2402,10 @@
         <v>50</v>
       </c>
       <c r="P27" t="s">
-        <v>212</v>
+        <v>197</v>
       </c>
       <c r="Q27" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
     </row>
     <row r="28" spans="1:17">
@@ -2496,7 +2496,7 @@
         <v>65</v>
       </c>
       <c r="P29" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="Q29" t="s">
         <v>30</v>
@@ -2540,7 +2540,7 @@
         <v>83</v>
       </c>
       <c r="P30" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="Q30" t="s">
         <v>30</v>
@@ -2587,7 +2587,7 @@
         <v>123</v>
       </c>
       <c r="P31" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="Q31" t="s">
         <v>30</v>
@@ -2631,7 +2631,7 @@
         <v>36</v>
       </c>
       <c r="P32" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
     </row>
     <row r="33" spans="1:17">
@@ -2672,7 +2672,7 @@
         <v>49</v>
       </c>
       <c r="P33" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
     </row>
     <row r="34" spans="1:17">
@@ -2716,7 +2716,7 @@
         <v>66</v>
       </c>
       <c r="P34" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
     </row>
     <row r="35" spans="1:17">
@@ -2760,7 +2760,7 @@
         <v>38</v>
       </c>
       <c r="Q35" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
     </row>
     <row r="36" spans="1:17">
@@ -2804,7 +2804,7 @@
         <v>38</v>
       </c>
       <c r="Q36" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
     </row>
     <row r="37" spans="1:17">
@@ -2851,7 +2851,7 @@
         <v>38</v>
       </c>
       <c r="Q37" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
     </row>
     <row r="38" spans="1:17">
@@ -2892,7 +2892,7 @@
         <v>35</v>
       </c>
       <c r="P38" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
     </row>
     <row r="39" spans="1:17">
@@ -2903,7 +2903,7 @@
         <v>916</v>
       </c>
       <c r="C39" t="s">
-        <v>184</v>
+        <v>207</v>
       </c>
       <c r="D39">
         <v>9</v>
@@ -2933,7 +2933,7 @@
         <v>65</v>
       </c>
       <c r="P39" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
     </row>
     <row r="40" spans="1:17">
@@ -2944,7 +2944,7 @@
         <v>916</v>
       </c>
       <c r="C40" t="s">
-        <v>185</v>
+        <v>208</v>
       </c>
       <c r="D40">
         <v>9</v>
@@ -2974,7 +2974,7 @@
         <v>65</v>
       </c>
       <c r="P40" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
     </row>
     <row r="41" spans="1:17">
@@ -2985,7 +2985,7 @@
         <v>917</v>
       </c>
       <c r="C41" t="s">
-        <v>186</v>
+        <v>209</v>
       </c>
       <c r="D41">
         <v>9</v>
@@ -3015,7 +3015,7 @@
         <v>55</v>
       </c>
       <c r="P41" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
     </row>
     <row r="42" spans="1:17">
@@ -3026,7 +3026,7 @@
         <v>917</v>
       </c>
       <c r="C42" t="s">
-        <v>187</v>
+        <v>210</v>
       </c>
       <c r="D42">
         <v>9</v>
@@ -3056,7 +3056,7 @@
         <v>55</v>
       </c>
       <c r="P42" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
     </row>
     <row r="43" spans="1:17">
@@ -3349,7 +3349,7 @@
         <v>34</v>
       </c>
       <c r="P49" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
     </row>
     <row r="50" spans="1:17">
@@ -3390,7 +3390,7 @@
         <v>68</v>
       </c>
       <c r="P50" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
     </row>
     <row r="51" spans="1:17">
@@ -3516,7 +3516,7 @@
         <v>60</v>
       </c>
       <c r="P53" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
     </row>
     <row r="54" spans="1:17">
@@ -3557,10 +3557,10 @@
         <v>95</v>
       </c>
       <c r="P54" t="s">
-        <v>214</v>
+        <v>199</v>
       </c>
       <c r="Q54" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
     </row>
     <row r="55" spans="1:17">
@@ -3601,10 +3601,10 @@
         <v>120</v>
       </c>
       <c r="P55" t="s">
-        <v>214</v>
+        <v>199</v>
       </c>
       <c r="Q55" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
     </row>
     <row r="56" spans="1:17">
@@ -3645,10 +3645,10 @@
         <v>35</v>
       </c>
       <c r="P56" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="Q56" t="s">
-        <v>211</v>
+        <v>196</v>
       </c>
     </row>
     <row r="57" spans="1:17">
@@ -3692,10 +3692,10 @@
         <v>70</v>
       </c>
       <c r="P57" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="Q57" t="s">
-        <v>211</v>
+        <v>196</v>
       </c>
     </row>
     <row r="58" spans="1:17">
@@ -3736,10 +3736,10 @@
         <v>75</v>
       </c>
       <c r="P58" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="Q58" t="s">
-        <v>211</v>
+        <v>196</v>
       </c>
     </row>
     <row r="59" spans="1:17">
@@ -3750,7 +3750,7 @@
         <v>934</v>
       </c>
       <c r="C59" t="s">
-        <v>183</v>
+        <v>211</v>
       </c>
       <c r="D59">
         <v>9</v>
@@ -3780,10 +3780,10 @@
         <v>100</v>
       </c>
       <c r="P59" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="Q59" t="s">
-        <v>211</v>
+        <v>196</v>
       </c>
     </row>
     <row r="60" spans="1:17">
@@ -3794,7 +3794,7 @@
         <v>934</v>
       </c>
       <c r="C60" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="D60">
         <v>9</v>
@@ -3824,10 +3824,10 @@
         <v>100</v>
       </c>
       <c r="P60" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="Q60" t="s">
-        <v>211</v>
+        <v>196</v>
       </c>
     </row>
     <row r="61" spans="1:17">
@@ -4085,10 +4085,10 @@
         <v>45</v>
       </c>
       <c r="P66" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="Q66" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
     </row>
     <row r="67" spans="1:17">
@@ -4129,10 +4129,10 @@
         <v>45</v>
       </c>
       <c r="P67" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="Q67" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
     </row>
     <row r="68" spans="1:17">
@@ -4176,7 +4176,7 @@
         <v>47</v>
       </c>
       <c r="P68" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
     </row>
     <row r="69" spans="1:17">
@@ -4220,7 +4220,7 @@
         <v>90</v>
       </c>
       <c r="P69" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
     </row>
     <row r="70" spans="1:17">
@@ -4261,7 +4261,7 @@
         <v>65</v>
       </c>
       <c r="P70" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
     </row>
     <row r="71" spans="1:17">
@@ -4302,7 +4302,7 @@
         <v>75</v>
       </c>
       <c r="P71" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="Q71" t="s">
         <v>53</v>
@@ -4316,7 +4316,7 @@
         <v>946</v>
       </c>
       <c r="C72" t="s">
-        <v>189</v>
+        <v>213</v>
       </c>
       <c r="D72">
         <v>9</v>
@@ -4346,7 +4346,7 @@
         <v>111</v>
       </c>
       <c r="P72" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="Q72" t="s">
         <v>53</v>
@@ -4360,7 +4360,7 @@
         <v>946</v>
       </c>
       <c r="C73" t="s">
-        <v>182</v>
+        <v>214</v>
       </c>
       <c r="D73">
         <v>9</v>
@@ -4390,7 +4390,7 @@
         <v>111</v>
       </c>
       <c r="P73" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="Q73" t="s">
         <v>53</v>
@@ -4434,7 +4434,7 @@
         <v>43</v>
       </c>
       <c r="P74" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
     </row>
     <row r="75" spans="1:17">
@@ -4475,7 +4475,7 @@
         <v>73</v>
       </c>
       <c r="P75" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
     </row>
     <row r="76" spans="1:17">
@@ -4522,7 +4522,7 @@
         <v>40</v>
       </c>
       <c r="Q76" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
     </row>
     <row r="77" spans="1:17">
@@ -4569,7 +4569,7 @@
         <v>40</v>
       </c>
       <c r="Q77" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
     </row>
     <row r="78" spans="1:17">
@@ -4616,7 +4616,7 @@
         <v>40</v>
       </c>
       <c r="Q78" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
     </row>
     <row r="79" spans="1:17">
@@ -4627,7 +4627,7 @@
         <v>952</v>
       </c>
       <c r="C79" t="s">
-        <v>190</v>
+        <v>215</v>
       </c>
       <c r="D79">
         <v>9</v>
@@ -4660,10 +4660,10 @@
         <v>82</v>
       </c>
       <c r="P79" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="Q79" t="s">
-        <v>211</v>
+        <v>196</v>
       </c>
     </row>
     <row r="80" spans="1:17">
@@ -4674,7 +4674,7 @@
         <v>952</v>
       </c>
       <c r="C80" t="s">
-        <v>191</v>
+        <v>216</v>
       </c>
       <c r="D80">
         <v>9</v>
@@ -4707,10 +4707,10 @@
         <v>82</v>
       </c>
       <c r="P80" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="Q80" t="s">
-        <v>211</v>
+        <v>196</v>
       </c>
     </row>
     <row r="81" spans="1:17">
@@ -4721,7 +4721,7 @@
         <v>952</v>
       </c>
       <c r="C81" t="s">
-        <v>192</v>
+        <v>217</v>
       </c>
       <c r="D81">
         <v>9</v>
@@ -4754,10 +4754,10 @@
         <v>82</v>
       </c>
       <c r="P81" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="Q81" t="s">
-        <v>211</v>
+        <v>196</v>
       </c>
     </row>
     <row r="82" spans="1:17">
@@ -4801,7 +4801,7 @@
         <v>121</v>
       </c>
       <c r="P82" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
     </row>
     <row r="83" spans="1:17">
@@ -4842,7 +4842,7 @@
         <v>60</v>
       </c>
       <c r="P83" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
     </row>
     <row r="84" spans="1:17">
@@ -4886,7 +4886,7 @@
         <v>85</v>
       </c>
       <c r="P84" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
     </row>
     <row r="85" spans="1:17">
@@ -4930,7 +4930,7 @@
         <v>105</v>
       </c>
       <c r="P85" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
     </row>
     <row r="86" spans="1:17">
@@ -4974,7 +4974,7 @@
         <v>70</v>
       </c>
       <c r="P86" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="Q86" t="s">
         <v>38</v>
@@ -5021,7 +5021,7 @@
         <v>125</v>
       </c>
       <c r="P87" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="Q87" t="s">
         <v>38</v>
@@ -5079,7 +5079,7 @@
         <v>960</v>
       </c>
       <c r="C89" t="s">
-        <v>193</v>
+        <v>218</v>
       </c>
       <c r="D89">
         <v>9</v>
@@ -5123,7 +5123,7 @@
         <v>960</v>
       </c>
       <c r="C90" t="s">
-        <v>194</v>
+        <v>219</v>
       </c>
       <c r="D90">
         <v>9</v>
@@ -5167,7 +5167,7 @@
         <v>960</v>
       </c>
       <c r="C91" t="s">
-        <v>195</v>
+        <v>220</v>
       </c>
       <c r="D91">
         <v>9</v>
@@ -5211,7 +5211,7 @@
         <v>960</v>
       </c>
       <c r="C92" t="s">
-        <v>196</v>
+        <v>221</v>
       </c>
       <c r="D92">
         <v>9</v>
@@ -5329,10 +5329,10 @@
         <v>75</v>
       </c>
       <c r="P94" t="s">
-        <v>214</v>
+        <v>199</v>
       </c>
       <c r="Q94" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
     </row>
     <row r="95" spans="1:17">
@@ -5373,7 +5373,7 @@
         <v>25</v>
       </c>
       <c r="P95" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
     </row>
     <row r="96" spans="1:17">
@@ -5414,7 +5414,7 @@
         <v>35</v>
       </c>
       <c r="P96" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
     </row>
     <row r="97" spans="1:17">
@@ -5455,7 +5455,7 @@
         <v>35</v>
       </c>
       <c r="P97" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
     </row>
     <row r="98" spans="1:17">
@@ -5499,7 +5499,7 @@
         <v>60</v>
       </c>
       <c r="P98" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
     </row>
     <row r="99" spans="1:17">
@@ -5543,7 +5543,7 @@
         <v>86</v>
       </c>
       <c r="P99" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
     </row>
     <row r="100" spans="1:17">
@@ -5587,7 +5587,7 @@
         <v>75</v>
       </c>
       <c r="P100" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
     </row>
     <row r="101" spans="1:17">
@@ -5631,7 +5631,7 @@
         <v>110</v>
       </c>
       <c r="P101" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
     </row>
     <row r="102" spans="1:17">
@@ -5672,10 +5672,10 @@
         <v>65</v>
       </c>
       <c r="P102" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="Q102" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
     </row>
     <row r="103" spans="1:17">
@@ -5716,10 +5716,10 @@
         <v>95</v>
       </c>
       <c r="P103" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="Q103" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
     </row>
     <row r="104" spans="1:17">
@@ -5760,7 +5760,7 @@
         <v>51</v>
       </c>
       <c r="P104" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
     </row>
     <row r="105" spans="1:17">
@@ -5801,7 +5801,7 @@
         <v>85</v>
       </c>
       <c r="P105" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
     </row>
     <row r="106" spans="1:17">
@@ -5900,7 +5900,7 @@
         <v>976</v>
       </c>
       <c r="C108" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="D108">
         <v>9</v>
@@ -5930,7 +5930,7 @@
         <v>10</v>
       </c>
       <c r="P108" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
     </row>
     <row r="109" spans="1:17">
@@ -5941,7 +5941,7 @@
         <v>976</v>
       </c>
       <c r="C109" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="D109">
         <v>9</v>
@@ -5971,7 +5971,7 @@
         <v>80</v>
       </c>
       <c r="P109" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
     </row>
     <row r="110" spans="1:17">
@@ -6015,7 +6015,7 @@
         <v>84</v>
       </c>
       <c r="P110" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
     </row>
     <row r="111" spans="1:17">
@@ -6059,7 +6059,7 @@
         <v>87</v>
       </c>
       <c r="P111" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
     </row>
     <row r="112" spans="1:17">
@@ -6103,7 +6103,7 @@
         <v>55</v>
       </c>
       <c r="P112" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
     </row>
     <row r="113" spans="1:16">
@@ -6114,7 +6114,7 @@
         <v>980</v>
       </c>
       <c r="C113" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="D113">
         <v>9</v>
@@ -6164,7 +6164,7 @@
         <v>101</v>
       </c>
       <c r="P114" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
     </row>
     <row r="115" spans="1:16">
@@ -6208,7 +6208,7 @@
         <v>111</v>
       </c>
       <c r="P115" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
     </row>
     <row r="116" spans="1:16">
@@ -6252,7 +6252,7 @@
         <v>135</v>
       </c>
       <c r="P116" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
     </row>
     <row r="117" spans="1:16">
@@ -6296,7 +6296,7 @@
         <v>81</v>
       </c>
       <c r="P117" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
     </row>
     <row r="118" spans="1:16">
@@ -6340,7 +6340,7 @@
         <v>119</v>
       </c>
       <c r="P118" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
     </row>
     <row r="119" spans="1:16">
@@ -6384,7 +6384,7 @@
         <v>106</v>
       </c>
       <c r="P119" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
     </row>
     <row r="120" spans="1:16">
@@ -6395,7 +6395,7 @@
         <v>987</v>
       </c>
       <c r="C120" t="s">
-        <v>200</v>
+        <v>185</v>
       </c>
       <c r="D120">
         <v>9</v>
@@ -6445,7 +6445,7 @@
         <v>110</v>
       </c>
       <c r="P121" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
     </row>
     <row r="122" spans="1:16">
@@ -6489,7 +6489,7 @@
         <v>50</v>
       </c>
       <c r="P122" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
     </row>
     <row r="123" spans="1:16">
@@ -6533,7 +6533,7 @@
         <v>108</v>
       </c>
       <c r="P123" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
     </row>
     <row r="124" spans="1:16">
@@ -6577,7 +6577,7 @@
         <v>72</v>
       </c>
       <c r="P124" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
     </row>
     <row r="125" spans="1:16">
@@ -6621,7 +6621,7 @@
         <v>136</v>
       </c>
       <c r="P125" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
     </row>
     <row r="126" spans="1:16">
@@ -6665,7 +6665,7 @@
         <v>116</v>
       </c>
       <c r="P126" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
     </row>
     <row r="127" spans="1:16">
@@ -6676,7 +6676,7 @@
         <v>994</v>
       </c>
       <c r="C127" t="s">
-        <v>218</v>
+        <v>203</v>
       </c>
       <c r="D127">
         <v>9</v>
@@ -6709,7 +6709,7 @@
         <v>45</v>
       </c>
       <c r="P127" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
     </row>
     <row r="128" spans="1:16">
@@ -6720,7 +6720,7 @@
         <v>995</v>
       </c>
       <c r="C128" t="s">
-        <v>219</v>
+        <v>204</v>
       </c>
       <c r="D128">
         <v>9</v>
@@ -6753,7 +6753,7 @@
         <v>135</v>
       </c>
       <c r="P128" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
     </row>
     <row r="129" spans="1:16">
@@ -6764,7 +6764,7 @@
         <v>996</v>
       </c>
       <c r="C129" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
       <c r="D129">
         <v>9</v>
@@ -6797,7 +6797,7 @@
         <v>70</v>
       </c>
       <c r="P129" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
     </row>
     <row r="130" spans="1:16">
@@ -6808,7 +6808,7 @@
         <v>997</v>
       </c>
       <c r="C130" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="D130">
         <v>9</v>
@@ -6841,7 +6841,7 @@
         <v>100</v>
       </c>
       <c r="P130" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
     </row>
     <row r="131" spans="1:16">
@@ -6885,7 +6885,7 @@
         <v>135</v>
       </c>
       <c r="P131" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
     </row>
     <row r="132" spans="1:16">
@@ -6929,7 +6929,7 @@
         <v>135</v>
       </c>
       <c r="P132" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
     </row>
     <row r="133" spans="1:16">
@@ -7102,7 +7102,7 @@
         <v>35</v>
       </c>
       <c r="P136" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
     </row>
     <row r="137" spans="1:16">
@@ -7146,7 +7146,7 @@
         <v>75</v>
       </c>
       <c r="P137" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
     </row>
     <row r="138" spans="1:16">
@@ -7190,7 +7190,7 @@
         <v>85</v>
       </c>
       <c r="P138" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
     </row>
     <row r="139" spans="1:16">
@@ -7322,7 +7322,7 @@
         <v>50</v>
       </c>
       <c r="P141" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
     </row>
     <row r="142" spans="1:16">
@@ -7366,7 +7366,7 @@
         <v>20</v>
       </c>
       <c r="P142" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
     </row>
     <row r="143" spans="1:16">
@@ -7410,7 +7410,7 @@
         <v>90</v>
       </c>
       <c r="P143" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
     </row>
     <row r="144" spans="1:16">
@@ -7421,7 +7421,7 @@
         <v>1011</v>
       </c>
       <c r="C144" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="D144">
         <v>9</v>
@@ -7438,7 +7438,7 @@
         <v>128</v>
       </c>
       <c r="C145" t="s">
-        <v>201</v>
+        <v>186</v>
       </c>
       <c r="D145">
         <v>9</v>
@@ -7468,7 +7468,7 @@
         <v>100</v>
       </c>
       <c r="P145" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
     </row>
     <row r="146" spans="1:17">
@@ -7479,7 +7479,7 @@
         <v>128</v>
       </c>
       <c r="C146" t="s">
-        <v>202</v>
+        <v>187</v>
       </c>
       <c r="D146">
         <v>9</v>
@@ -7512,7 +7512,7 @@
         <v>100</v>
       </c>
       <c r="P146" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
     </row>
     <row r="147" spans="1:17">
@@ -7523,7 +7523,7 @@
         <v>128</v>
       </c>
       <c r="C147" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="D147">
         <v>9</v>
@@ -7556,7 +7556,7 @@
         <v>100</v>
       </c>
       <c r="P147" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
     </row>
     <row r="148" spans="1:17">
@@ -7600,10 +7600,10 @@
         <v>15</v>
       </c>
       <c r="P148" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="Q148" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: adjust for change family to line
</commit_message>
<xml_diff>
--- a/data/pokemon_dex_hisui_paldea.xlsx
+++ b/data/pokemon_dex_hisui_paldea.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\panpa\Google Drive\Data science\pkmr\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30D6C972-5198-40FD-8FDC-EEF954163001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84BA7A0E-7D46-4AB3-9FEB-D809ED35A403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1245" yWindow="30" windowWidth="19245" windowHeight="11490" xr2:uid="{B1A15022-E2F9-4772-961C-F274C4B8A95E}"/>
+    <workbookView xWindow="825" yWindow="-120" windowWidth="19785" windowHeight="11760" xr2:uid="{B1A15022-E2F9-4772-961C-F274C4B8A95E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1054,8 +1054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5180E553-97C3-4D11-A13B-DD8E8ABEE531}">
   <dimension ref="A1:Q148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="C93" sqref="C93"/>
+    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>

</xml_diff>